<commit_message>
add amogus to dataBase
</commit_message>
<xml_diff>
--- a/img/data.xlsx
+++ b/img/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuatr\Desktop\tgboot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cuatr\Desktop\meme-bot\img\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659A6FFD-A9C8-4AF5-8ECF-AD6CBFB807D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42043EB7-527A-4ECA-B9AF-7AADC0E7EF37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="2016" windowWidth="7500" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13308" yWindow="1980" windowWidth="7500" windowHeight="8220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <t>сейчас проведем вам высокоскоростной интернет будете зарабатывать в сети репутацию долбаеба кот котик лестница кабель провод</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>амогус раскраска на изи амонг ас амонгас amogus among us amongus lol лол impostor импостер веселые картинки круто новинка kek кек</t>
   </si>
 </sst>
 </file>
@@ -914,7 +914,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -947,7 +947,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>

</xml_diff>